<commit_message>
GH Action: Update Pilot 5 ECTD bundle
</commit_message>
<xml_diff>
--- a/m5/datasets/rconsortiumpilot5/analysis/adam/datasets/adam-pilot-5.xlsx
+++ b/m5/datasets/rconsortiumpilot5/analysis/adam/datasets/adam-pilot-5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cp903461\Downloads\datasetJSON Pilot 5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bs832471\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B7D320-95C3-48CA-8A87-AB3E1A927A48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF11C82C-F6EF-413B-89BD-15DA31EDCD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Define" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ValueLevel!$A$1:$R$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Variables!$A$1:$S$217</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5057" uniqueCount="1222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5055" uniqueCount="1223">
   <si>
     <t>Attribute</t>
   </si>
@@ -3729,17 +3729,34 @@
   </si>
   <si>
     <t>StandardVersion</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3815,20 +3832,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -8338,9 +8359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L75" sqref="L75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9304,12 +9325,10 @@
       <c r="E28" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="F28" s="5">
+        <v>8</v>
+      </c>
+      <c r="G28" s="5"/>
       <c r="H28" s="5"/>
       <c r="I28" s="2" t="s">
         <v>27</v>
@@ -9336,11 +9355,12 @@
         <v>184</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="G29" s="10"/>
       <c r="H29" s="5"/>
       <c r="I29" s="2" t="s">
         <v>27</v>
@@ -9367,11 +9387,12 @@
         <v>188</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>83</v>
       </c>
+      <c r="G30" s="10"/>
       <c r="H30" s="5"/>
       <c r="I30" s="2" t="s">
         <v>27</v>
@@ -9398,7 +9419,7 @@
         <v>192</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>83</v>
@@ -17890,7 +17911,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -17984,14 +18005,14 @@
       <c r="E2" s="2" t="s">
         <v>593</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>115</v>
+      <c r="G2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>27</v>
@@ -18019,14 +18040,14 @@
       <c r="E3" s="2" t="s">
         <v>595</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>115</v>
+      <c r="G3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>27</v>
@@ -18054,14 +18075,14 @@
       <c r="E4" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>115</v>
+      <c r="G4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>27</v>
@@ -18089,14 +18110,14 @@
       <c r="E5" s="2" t="s">
         <v>599</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>115</v>
+      <c r="G5" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>27</v>
@@ -18124,14 +18145,14 @@
       <c r="E6" s="2" t="s">
         <v>601</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>115</v>
+      <c r="G6" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>27</v>
@@ -18159,14 +18180,14 @@
       <c r="E7" s="2" t="s">
         <v>603</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>115</v>
+      <c r="G7" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>27</v>
@@ -18194,14 +18215,14 @@
       <c r="E8" s="2" t="s">
         <v>605</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>115</v>
+      <c r="G8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>27</v>
@@ -18229,14 +18250,14 @@
       <c r="E9" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>115</v>
+      <c r="G9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>27</v>
@@ -18264,14 +18285,14 @@
       <c r="E10" s="2" t="s">
         <v>609</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>115</v>
+      <c r="G10" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>27</v>
@@ -18299,14 +18320,14 @@
       <c r="E11" s="2" t="s">
         <v>611</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>115</v>
+      <c r="G11" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>27</v>
@@ -18334,14 +18355,14 @@
       <c r="E12" s="2" t="s">
         <v>613</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>115</v>
+      <c r="G12" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>27</v>
@@ -18369,14 +18390,14 @@
       <c r="E13" s="2" t="s">
         <v>615</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>115</v>
+      <c r="G13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J13" s="2" t="s">
         <v>27</v>
@@ -18404,14 +18425,14 @@
       <c r="E14" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>115</v>
+      <c r="G14" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>27</v>
@@ -18439,14 +18460,14 @@
       <c r="E15" s="2" t="s">
         <v>619</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>115</v>
+      <c r="G15" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>27</v>
@@ -18474,14 +18495,14 @@
       <c r="E16" s="2" t="s">
         <v>621</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>115</v>
+      <c r="G16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>1222</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>27</v>
@@ -19485,7 +19506,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView zoomScale="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B64" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B318" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="F74" sqref="F74"/>
@@ -28139,7 +28160,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:H983"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
     </sheetView>

</xml_diff>